<commit_message>
LW155 W&TCV import and import of the schedule documents. Also am now always switching imported documents to character to avoid a date error on join.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/SM-3 BLOCK IIA/SM-3 IIA Schedule Info.xlsx
+++ b/FOIA SAR data/SM-3 BLOCK IIA/SM-3 IIA Schedule Info.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2007-01 PROFESSIONAL SERVICES\R scripts and data\FOIA SAR data\SM-3 BLOCK IIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\R-scripts-and-data\FOIA SAR data\SM-3 BLOCK IIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -247,13 +247,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,11 +651,11 @@
       <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -883,11 +883,11 @@
       <c r="B24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
@@ -1029,183 +1029,180 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G36" t="s">
-        <v>36</v>
-      </c>
-      <c r="H36" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>27</v>
+      <c r="A37" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>28</v>
+      <c r="A38" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>33</v>
+      <c r="A39" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>40</v>
+      <c r="A41" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" t="s">
-        <v>37</v>
-      </c>
-      <c r="H46" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>2015</v>
       </c>
     </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" t="s">
+        <v>43</v>
+      </c>
+      <c r="H51" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D52" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E52" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" t="s">
-        <v>37</v>
-      </c>
-      <c r="G52" t="s">
-        <v>43</v>
-      </c>
-      <c r="H52" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" t="s">
-        <v>47</v>
-      </c>
-      <c r="E53" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>